<commit_message>
Added new link to MIT lecture
</commit_message>
<xml_diff>
--- a/Useful Links.xlsx
+++ b/Useful Links.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>ML Course Wiki</t>
   </si>
@@ -36,6 +36,9 @@
   </si>
   <si>
     <t>https://www.coursera.org/learn/machine-learning/discussions/m0ZdvjSrEeWddiIAC9pDDA</t>
+  </si>
+  <si>
+    <t>Explanation of Back Propagation</t>
   </si>
 </sst>
 </file>
@@ -350,10 +353,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -378,6 +381,11 @@
         <v>3</v>
       </c>
     </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added useful links on neural networks
</commit_message>
<xml_diff>
--- a/Useful Links.xlsx
+++ b/Useful Links.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26124"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26207"/>
   <workbookPr showInkAnnotation="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>ML Course Wiki</t>
   </si>
@@ -38,7 +38,16 @@
     <t>https://www.coursera.org/learn/machine-learning/discussions/m0ZdvjSrEeWddiIAC9pDDA</t>
   </si>
   <si>
-    <t>Explanation of Back Propagation</t>
+    <t>https://www.youtube.com/watch?v=q0pm3BrIUFo</t>
+  </si>
+  <si>
+    <t>Explanations of Back Propagation</t>
+  </si>
+  <si>
+    <t>http://ocw.mit.edu/courses/electrical-engineering-and-computer-science/6-034-artificial-intelligence-fall-2010/readings/MIT6_034F10_netmath.pdf</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=Ih5Mr93E-2c&amp;hd=1</t>
   </si>
 </sst>
 </file>
@@ -353,15 +362,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="20.33203125" customWidth="1"/>
+    <col min="1" max="1" width="27.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="55" customWidth="1"/>
   </cols>
   <sheetData>
@@ -383,7 +392,20 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
         <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B5" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added a bunch of useful links
</commit_message>
<xml_diff>
--- a/Useful Links.xlsx
+++ b/Useful Links.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>ML Course Wiki</t>
   </si>
@@ -48,6 +48,36 @@
   </si>
   <si>
     <t>https://www.youtube.com/watch?v=Ih5Mr93E-2c&amp;hd=1</t>
+  </si>
+  <si>
+    <t>Intro to Statistical Learning ebook</t>
+  </si>
+  <si>
+    <t>http://www-bcf.usc.edu/~gareth/ISL/ISLR%20Fourth%20Printing.pdf</t>
+  </si>
+  <si>
+    <t>http://www.alsharif.info/#!iom530/c21o7</t>
+  </si>
+  <si>
+    <t>Intro to Statistical Learning website</t>
+  </si>
+  <si>
+    <t>http://www-bcf.usc.edu/~gareth/ISL/</t>
+  </si>
+  <si>
+    <t>Intro to Statistical Learning MOOC</t>
+  </si>
+  <si>
+    <t>Applied statistical learning techniques (Slides and tuts)</t>
+  </si>
+  <si>
+    <t>http://www.r-bloggers.com/in-depth-introduction-to-machine-learning-in-15-hours-of-expert-videos/</t>
+  </si>
+  <si>
+    <t>Intro to Statistical Learning Stanford MOOC (Course)</t>
+  </si>
+  <si>
+    <t>https://lagunita.stanford.edu/courses/HumanitiesScience/StatLearning/Winter2014/about</t>
   </si>
 </sst>
 </file>
@@ -362,16 +392,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="27.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="55" customWidth="1"/>
+    <col min="1" max="1" width="48.5" customWidth="1"/>
+    <col min="2" max="2" width="163.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
@@ -408,6 +438,46 @@
         <v>7</v>
       </c>
     </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" t="s">
+        <v>17</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>